<commit_message>
stuck on getting values from csv
</commit_message>
<xml_diff>
--- a/testFiles/resident.xlsx
+++ b/testFiles/resident.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/estevenson/Door-Deck-Creator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\Desktop\Code\Door-Deck-Creator\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{172D69E7-2736-754B-8E4F-97F6CD8D0849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6FC1CE-78FB-44AE-A2C1-E65986D80D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16480" xr2:uid="{15F428D2-5C0A-FF48-8D09-299E6A8C157E}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{15F428D2-5C0A-FF48-8D09-299E6A8C157E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -483,15 +483,15 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -507,7 +507,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -515,7 +515,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -523,7 +523,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -531,7 +531,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -539,7 +539,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -547,7 +547,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -555,7 +555,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -563,7 +563,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -571,7 +571,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -579,7 +579,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -587,7 +587,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -595,7 +595,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -603,7 +603,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -611,7 +611,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -619,7 +619,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -627,7 +627,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -635,7 +635,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -643,7 +643,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -651,7 +651,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -659,7 +659,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -667,7 +667,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -675,7 +675,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -683,7 +683,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -691,7 +691,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -699,7 +699,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -707,7 +707,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -715,7 +715,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>

</xml_diff>